<commit_message>
Hybrid and testng framework changed
</commit_message>
<xml_diff>
--- a/src/test/resources/Test Suite1.xlsx
+++ b/src/test/resources/Test Suite1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1215" windowWidth="16785" windowHeight="3450" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="1215" windowWidth="16785" windowHeight="3450" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Test Data" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A5:K14"/>
+  <oleSize ref="A1:G10"/>
 </workbook>
 </file>
 
@@ -600,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -923,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1009,7 +1009,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
pom file changes and added the new test cases.
</commit_message>
<xml_diff>
--- a/src/test/resources/Test Suite1.xlsx
+++ b/src/test/resources/Test Suite1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1215" windowWidth="16785" windowHeight="3450" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="1155" windowWidth="16785" windowHeight="3510" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="Test Data" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:G10"/>
+  <oleSize ref="A19:K28"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="92">
   <si>
     <t>TCID</t>
   </si>
@@ -157,13 +157,142 @@
     <t>vetrivel@gmail.com</t>
   </si>
   <si>
-    <t>956565635</t>
-  </si>
-  <si>
     <t>1234567</t>
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>BrokenLinkTest</t>
+  </si>
+  <si>
+    <t>Check the broken link in HousingMan desktop and Mobile site</t>
+  </si>
+  <si>
+    <t>linkCheck</t>
+  </si>
+  <si>
+    <t>checkNavigateURL</t>
+  </si>
+  <si>
+    <t>Authorized|URL</t>
+  </si>
+  <si>
+    <t>JavaScriptPagination</t>
+  </si>
+  <si>
+    <t>checkPagination</t>
+  </si>
+  <si>
+    <t>N|http://54.169.220.31/</t>
+  </si>
+  <si>
+    <t>N|http://54.169.220.31/projects?utf8=%E2%9C%93&amp;city_id=bangalore&amp;q=&amp;search_filter%5Bsales_type_any%5D%5B%5D=new&amp;keywords=&amp;search_filter%5Bprice_range_any%5D%5B%5D=&amp;search_filter%5Bprice_range_any%5D%5B%5D=</t>
+  </si>
+  <si>
+    <t>projectNameLink|footerPage1Link|footerPage2Link</t>
+  </si>
+  <si>
+    <t>Y|http://54.169.220.31</t>
+  </si>
+  <si>
+    <t>N|http://54.169.220.31/projects/birundha-apartments</t>
+  </si>
+  <si>
+    <t>N|http://54.169.220.31/builders/the-rocking-bangalore-groups-of-apartments</t>
+  </si>
+  <si>
+    <t>N|http://54.169.220.31/credai-builders-in-bangalore</t>
+  </si>
+  <si>
+    <t>N|http://52.77.215.120/credai-apartments-in-bangalore</t>
+  </si>
+  <si>
+    <t>567</t>
+  </si>
+  <si>
+    <t>drjames@ymail.com</t>
+  </si>
+  <si>
+    <t>Letters and space allowed</t>
+  </si>
+  <si>
+    <t>Arun</t>
+  </si>
+  <si>
+    <t>That</t>
+  </si>
+  <si>
+    <t>sathish@gmail</t>
+  </si>
+  <si>
+    <t>Sathish</t>
+  </si>
+  <si>
+    <t>Arun Balaji</t>
+  </si>
+  <si>
+    <t>arun_balaji@gmail.com</t>
+  </si>
+  <si>
+    <t>Jaykanth</t>
+  </si>
+  <si>
+    <t>jaykanth234@gmail.com</t>
+  </si>
+  <si>
+    <t>hjdjdjnsj</t>
+  </si>
+  <si>
+    <t>Enter the valid mobile number</t>
+  </si>
+  <si>
+    <t>Enter the valid email</t>
+  </si>
+  <si>
+    <t>9916452518</t>
+  </si>
+  <si>
+    <t>Mobile number is already exist</t>
+  </si>
+  <si>
+    <t>Jakay</t>
+  </si>
+  <si>
+    <t>Email is already exist</t>
+  </si>
+  <si>
+    <t>Dhoni</t>
+  </si>
+  <si>
+    <t>dhoni@gmail.com</t>
+  </si>
+  <si>
+    <t>9565656352</t>
+  </si>
+  <si>
+    <t>9565656354</t>
+  </si>
+  <si>
+    <t>9565656358</t>
+  </si>
+  <si>
+    <t>9565656351</t>
+  </si>
+  <si>
+    <t>Password field should be 8_digit letters</t>
+  </si>
+  <si>
+    <t>waitUtilFind</t>
+  </si>
+  <si>
+    <t>check_Out_btn</t>
+  </si>
+  <si>
+    <t>Search_ListingPage</t>
+  </si>
+  <si>
+    <t>Verity the all project and count in search listing page.</t>
   </si>
 </sst>
 </file>
@@ -212,7 +341,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -235,6 +364,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -243,13 +383,14 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -545,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -588,6 +729,28 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -598,10 +761,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -609,7 +772,7 @@
     <col min="1" max="1" width="18" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="33" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="16.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -852,7 +1015,7 @@
         <v>33</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -912,6 +1075,130 @@
         <v>37</v>
       </c>
       <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -921,16 +1208,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="22.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="24.140625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="19.85546875" customWidth="1" collapsed="1"/>
@@ -1022,7 +1310,9 @@
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -1035,7 +1325,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>11</v>
@@ -1060,22 +1350,281 @@
       <c r="B12" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" t="s">
         <v>45</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>47</v>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1"/>
-    <hyperlink ref="C12" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>